<commit_message>
Changelog, and Ore Distribution spreadsheet now has Deep Dark ores
</commit_message>
<xml_diff>
--- a/Documents/OreDistribution.xlsx
+++ b/Documents/OreDistribution.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nether" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Deep Dark" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -124,6 +125,117 @@
   </si>
   <si>
     <t>Nether</t>
+  </si>
+  <si>
+    <t>Deep Dark</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Fe-Cu-Sn Mix</t>
+  </si>
+  <si>
+    <t>Mana Infused</t>
+  </si>
+  <si>
+    <t>Prometheum</t>
+  </si>
+  <si>
+    <t>Deep Iron</t>
+  </si>
+  <si>
+    <t>Infuscolium</t>
+  </si>
+  <si>
+    <t>Oureclase</t>
+  </si>
+  <si>
+    <t>Astral Silver</t>
+  </si>
+  <si>
+    <t>Carmot</t>
+  </si>
+  <si>
+    <t>Mithril</t>
+  </si>
+  <si>
+    <t>Rubracium</t>
+  </si>
+  <si>
+    <t>Orichalcum</t>
+  </si>
+  <si>
+    <t>Adamantine</t>
+  </si>
+  <si>
+    <t>Atlarus</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Certus Quartz</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Manganese</t>
+  </si>
+  <si>
+    <t>Sulfur - Veins</t>
+  </si>
+  <si>
+    <t>Sulfur - Deposits</t>
+  </si>
+  <si>
+    <t>Apatite</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Redstone</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Lapis</t>
+  </si>
+  <si>
+    <t>Emerald</t>
+  </si>
+  <si>
+    <t>Bitumen</t>
+  </si>
+  <si>
+    <t>Potash</t>
+  </si>
+  <si>
+    <t>Saltpeter</t>
+  </si>
+  <si>
+    <t>Posphorite</t>
   </si>
 </sst>
 </file>
@@ -850,8 +962,8 @@
             </c:spPr>
           </c:downBars>
         </c:upDownBars>
-        <c:axId val="288326824"/>
-        <c:axId val="288322512"/>
+        <c:axId val="318744600"/>
+        <c:axId val="318741464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1155,7 +1267,7 @@
         </c:extLst>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="288326824"/>
+        <c:axId val="318744600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288322512"/>
+        <c:crossAx val="318741464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1220,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288322512"/>
+        <c:axId val="318741464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="128"/>
@@ -1284,7 +1396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288326824"/>
+        <c:crossAx val="318744600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="32"/>
@@ -1318,6 +1430,1365 @@
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Deep Dark</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$G$3:$G$42</c:f>
+              <c:strCache>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>Copper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Silver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lead</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Nickel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Osmium</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fe-Cu-Sn Mix</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mana Infused</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Prometheum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Deep Iron</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Infuscolium</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Oureclase</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Astral Silver</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Carmot</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mithril</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Rubracium</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Orichalcum</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Adamantine</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Atlarus</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Platinum</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Zinc</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Certus Quartz</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Aluminum</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Manganese</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Sulfur - Veins</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Sulfur - Deposits</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Apatite</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Salt</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Coal</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Iron</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Gold</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Redstone</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Diamond</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Lapis</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Emerald</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Magnesium</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Bitumen</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Potash</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Saltpeter</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Posphorite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$H$3:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$G$3:$G$42</c:f>
+              <c:strCache>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>Copper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Silver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lead</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Nickel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Osmium</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fe-Cu-Sn Mix</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mana Infused</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Prometheum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Deep Iron</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Infuscolium</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Oureclase</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Astral Silver</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Carmot</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mithril</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Rubracium</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Orichalcum</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Adamantine</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Atlarus</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Platinum</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Zinc</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Certus Quartz</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Aluminum</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Manganese</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Sulfur - Veins</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Sulfur - Deposits</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Apatite</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Salt</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Coal</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Iron</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Gold</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Redstone</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Diamond</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Lapis</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Emerald</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Magnesium</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Bitumen</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Potash</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Saltpeter</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Posphorite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$3:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="362214184"/>
+        <c:axId val="362213008"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$J$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Mean</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="8"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$G$3:$G$42</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="40"/>
+                      <c:pt idx="0">
+                        <c:v>Copper</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Tin</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Silver</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lead</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Nickel</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Osmium</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Fe-Cu-Sn Mix</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Mana Infused</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Prometheum</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Deep Iron</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>Infuscolium</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Oureclase</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>Astral Silver</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>Carmot</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>Mithril</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>Rubracium</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>Orichalcum</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>Adamantine</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>Atlarus</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>Platinum</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>Zinc</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>Certus Quartz</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>Aluminum</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>Manganese</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>Sulfur - Veins</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Sulfur - Deposits</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Apatite</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>Salt</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>Coal</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>Iron</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>Gold</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>Redstone</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>Diamond</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>Lapis</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>Emerald</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>Magnesium</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>Bitumen</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>Potash</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>Saltpeter</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>Posphorite</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$J$3:$J$42</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="40"/>
+                      <c:pt idx="0">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>22.5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>169</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>228.5</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>234.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>224.5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>228.5</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>242</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>243</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>233</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>219</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>239.5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>247</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>241.5</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>62.5</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>141</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>157</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>139.5</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>11.5</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>127.5</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>177.5</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>127.5</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>110</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="362214184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="35000"/>
+                <a:lumOff val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362213008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362213008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="260"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362214184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="32"/>
+        <c:minorUnit val="16"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="45000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="56500">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="83000"/>
+                <a:lumOff val="17000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="71000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1399,6 +2870,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
   <cs:axisTitle>
@@ -1930,6 +3441,537 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1948,6 +3990,43 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2232,7 +4311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2243,10 +4322,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,14 +4346,18 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2274,8 +4370,20 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2289,8 +4397,21 @@
         <f>AVERAGE(B3:B3)</f>
         <v>88</v>
       </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>66</v>
+      </c>
+      <c r="I3">
+        <v>84</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE(H3:I3)</f>
+        <v>75</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2304,8 +4425,21 @@
         <f>AVERAGE(B4:B4)</f>
         <v>64</v>
       </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>66</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J42" si="0">AVERAGE(H4:I4)</f>
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2319,8 +4453,21 @@
         <f>AVERAGE(B5:B5)</f>
         <v>64</v>
       </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>29</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2334,8 +4481,21 @@
         <f>AVERAGE(B6:B6)</f>
         <v>16</v>
       </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2346,11 +4506,24 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D4:D30" si="0">AVERAGE(B7:C7)</f>
+        <f t="shared" ref="D7:D30" si="1">AVERAGE(B7:C7)</f>
         <v>32</v>
       </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2361,11 +4534,24 @@
         <v>54</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>39</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2376,11 +4562,24 @@
         <v>16</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>84</v>
+      </c>
+      <c r="I9">
+        <v>254</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2391,11 +4590,24 @@
         <v>68</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2406,11 +4618,24 @@
         <v>60</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11">
+        <v>215</v>
+      </c>
+      <c r="I11">
+        <v>242</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>228.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2421,11 +4646,24 @@
         <v>32</v>
       </c>
       <c r="D12">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12">
+        <v>223</v>
+      </c>
+      <c r="I12">
+        <v>246</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>234.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2436,263 +4674,677 @@
         <v>102</v>
       </c>
       <c r="D13">
+        <f t="shared" si="1"/>
+        <v>62.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <v>208</v>
+      </c>
+      <c r="I13">
+        <v>241</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>224.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>96</v>
+      </c>
+      <c r="C14">
+        <v>126</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14">
+        <v>208</v>
+      </c>
+      <c r="I14">
+        <v>249</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>228.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15">
+        <v>235</v>
+      </c>
+      <c r="I15">
+        <v>249</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>58</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>235</v>
+      </c>
+      <c r="I16">
+        <v>251</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>122</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17">
+        <v>221</v>
+      </c>
+      <c r="I17">
+        <v>245</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18">
+        <v>208</v>
+      </c>
+      <c r="I18">
+        <v>230</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19">
+        <v>230</v>
+      </c>
+      <c r="I19">
+        <v>249</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>239.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>126</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20">
+        <v>242</v>
+      </c>
+      <c r="I20">
+        <v>252</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>66</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>234</v>
+      </c>
+      <c r="I21">
+        <v>249</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>241.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>66</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23">
+        <v>55</v>
+      </c>
+      <c r="I23">
+        <v>75</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>48</v>
+      </c>
+      <c r="C24">
+        <v>76</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24">
+        <v>36</v>
+      </c>
+      <c r="I24">
+        <v>70</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>122</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>63.5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25">
+        <v>44</v>
+      </c>
+      <c r="I25">
+        <v>81</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>96</v>
-      </c>
-      <c r="C14">
-        <v>126</v>
-      </c>
-      <c r="D14">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>66</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26">
+        <v>56</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="0"/>
-        <v>111</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>52</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27">
+        <v>136</v>
+      </c>
+      <c r="I27">
+        <v>146</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>66</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>13</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>33.5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29">
+        <v>45</v>
+      </c>
+      <c r="I29">
+        <v>83</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
         <v>12</v>
       </c>
-      <c r="C15">
-        <v>56</v>
-      </c>
-      <c r="D15">
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30">
+        <v>60</v>
+      </c>
+      <c r="I30">
+        <v>254</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>58</v>
-      </c>
-      <c r="D16">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31">
+        <v>24</v>
+      </c>
+      <c r="I31">
+        <v>255</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>139.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>70</v>
-      </c>
-      <c r="C17">
-        <v>122</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>24</v>
-      </c>
-      <c r="C18">
-        <v>48</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>32</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>48</v>
-      </c>
-      <c r="C20">
-        <v>126</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>38</v>
-      </c>
-      <c r="C21">
-        <v>66</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>52</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>38</v>
-      </c>
-      <c r="C23">
-        <v>66</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>48</v>
-      </c>
-      <c r="C24">
-        <v>76</v>
-      </c>
-      <c r="D24">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32">
+        <v>45</v>
+      </c>
+      <c r="I32">
+        <v>79</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>122</v>
-      </c>
-      <c r="D25">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+      <c r="I33">
+        <v>31</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34">
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <v>23</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>20</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>21</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>105</v>
+      </c>
+      <c r="I38">
+        <v>150</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
         <v>66</v>
       </c>
-      <c r="D26">
+      <c r="H39">
+        <v>105</v>
+      </c>
+      <c r="I39">
+        <v>250</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>177.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27">
-        <v>24</v>
-      </c>
-      <c r="C27">
-        <v>52</v>
-      </c>
-      <c r="D27">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>67</v>
+      </c>
+      <c r="H40">
+        <v>105</v>
+      </c>
+      <c r="I40">
+        <v>150</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>127.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>38</v>
-      </c>
-      <c r="C28">
-        <v>66</v>
-      </c>
-      <c r="D28">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>128</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>29</v>
-      </c>
-      <c r="C29">
-        <v>38</v>
-      </c>
-      <c r="D29">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42">
+        <v>85</v>
+      </c>
+      <c r="I42">
+        <v>135</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="0"/>
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>12</v>
-      </c>
-      <c r="C30">
-        <v>24</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed duplicate Mithril from World Gen Thermal Foundation Mana-Infused ore is Mithril in disguise. Mana-Infused ore gen was disabled, and Metallurgy Mirthril gen was adjusted
</commit_message>
<xml_diff>
--- a/Documents/OreDistribution.xlsx
+++ b/Documents/OreDistribution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Nether" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Fe-Cu-Sn Mix</t>
-  </si>
-  <si>
-    <t>Mana Infused</t>
   </si>
   <si>
     <t>Prometheum</t>
@@ -962,8 +959,8 @@
             </c:spPr>
           </c:downBars>
         </c:upDownBars>
-        <c:axId val="318744600"/>
-        <c:axId val="318741464"/>
+        <c:axId val="308118872"/>
+        <c:axId val="308116912"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1267,7 +1264,7 @@
         </c:extLst>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="318744600"/>
+        <c:axId val="308118872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318741464"/>
+        <c:crossAx val="308116912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1332,7 +1329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318741464"/>
+        <c:axId val="308116912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="128"/>
@@ -1396,7 +1393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318744600"/>
+        <c:crossAx val="308118872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="32"/>
@@ -1628,9 +1625,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$G$3:$G$42</c:f>
+              <c:f>Data!$G$3:$G$41</c:f>
               <c:strCache>
-                <c:ptCount val="40"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Copper</c:v>
                 </c:pt>
@@ -1653,102 +1650,99 @@
                   <c:v>Fe-Cu-Sn Mix</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Mana Infused</c:v>
+                  <c:v>Prometheum</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Prometheum</c:v>
+                  <c:v>Deep Iron</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Deep Iron</c:v>
+                  <c:v>Infuscolium</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Infuscolium</c:v>
+                  <c:v>Oureclase</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Oureclase</c:v>
+                  <c:v>Astral Silver</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Astral Silver</c:v>
+                  <c:v>Carmot</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Carmot</c:v>
+                  <c:v>Mithril</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Mithril</c:v>
+                  <c:v>Rubracium</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Rubracium</c:v>
+                  <c:v>Orichalcum</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Orichalcum</c:v>
+                  <c:v>Adamantine</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Adamantine</c:v>
+                  <c:v>Atlarus</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Atlarus</c:v>
+                  <c:v>Platinum</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Platinum</c:v>
+                  <c:v>Zinc</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Zinc</c:v>
+                  <c:v>Certus Quartz</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Certus Quartz</c:v>
+                  <c:v>Aluminum</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Aluminum</c:v>
+                  <c:v>Manganese</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Manganese</c:v>
+                  <c:v>Sulfur - Veins</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Sulfur - Veins</c:v>
+                  <c:v>Sulfur - Deposits</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Sulfur - Deposits</c:v>
+                  <c:v>Apatite</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Apatite</c:v>
+                  <c:v>Salt</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Salt</c:v>
+                  <c:v>Coal</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Coal</c:v>
+                  <c:v>Iron</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Iron</c:v>
+                  <c:v>Gold</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Gold</c:v>
+                  <c:v>Redstone</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Redstone</c:v>
+                  <c:v>Diamond</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Diamond</c:v>
+                  <c:v>Lapis</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Lapis</c:v>
+                  <c:v>Emerald</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Emerald</c:v>
+                  <c:v>Magnesium</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Magnesium</c:v>
+                  <c:v>Bitumen</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Bitumen</c:v>
+                  <c:v>Potash</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Potash</c:v>
+                  <c:v>Saltpeter</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>Saltpeter</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>Posphorite</c:v>
                 </c:pt>
               </c:strCache>
@@ -1756,10 +1750,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$H$3:$H$42</c:f>
+              <c:f>Data!$H$3:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>66</c:v>
                 </c:pt>
@@ -1782,79 +1776,79 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>215</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>223</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>208</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>235</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>221</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>208</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>230</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>242</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>234</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>136</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>2</c:v>
@@ -1863,7 +1857,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>105</c:v>
@@ -1872,12 +1866,9 @@
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>105</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
@@ -1968,9 +1959,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$G$3:$G$42</c:f>
+              <c:f>Data!$G$3:$G$41</c:f>
               <c:strCache>
-                <c:ptCount val="40"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Copper</c:v>
                 </c:pt>
@@ -1993,102 +1984,99 @@
                   <c:v>Fe-Cu-Sn Mix</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Mana Infused</c:v>
+                  <c:v>Prometheum</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Prometheum</c:v>
+                  <c:v>Deep Iron</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Deep Iron</c:v>
+                  <c:v>Infuscolium</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Infuscolium</c:v>
+                  <c:v>Oureclase</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Oureclase</c:v>
+                  <c:v>Astral Silver</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Astral Silver</c:v>
+                  <c:v>Carmot</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Carmot</c:v>
+                  <c:v>Mithril</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Mithril</c:v>
+                  <c:v>Rubracium</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Rubracium</c:v>
+                  <c:v>Orichalcum</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Orichalcum</c:v>
+                  <c:v>Adamantine</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Adamantine</c:v>
+                  <c:v>Atlarus</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Atlarus</c:v>
+                  <c:v>Platinum</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Platinum</c:v>
+                  <c:v>Zinc</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Zinc</c:v>
+                  <c:v>Certus Quartz</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Certus Quartz</c:v>
+                  <c:v>Aluminum</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Aluminum</c:v>
+                  <c:v>Manganese</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Manganese</c:v>
+                  <c:v>Sulfur - Veins</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Sulfur - Veins</c:v>
+                  <c:v>Sulfur - Deposits</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Sulfur - Deposits</c:v>
+                  <c:v>Apatite</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Apatite</c:v>
+                  <c:v>Salt</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Salt</c:v>
+                  <c:v>Coal</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Coal</c:v>
+                  <c:v>Iron</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Iron</c:v>
+                  <c:v>Gold</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Gold</c:v>
+                  <c:v>Redstone</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Redstone</c:v>
+                  <c:v>Diamond</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Diamond</c:v>
+                  <c:v>Lapis</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Lapis</c:v>
+                  <c:v>Emerald</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Emerald</c:v>
+                  <c:v>Magnesium</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Magnesium</c:v>
+                  <c:v>Bitumen</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Bitumen</c:v>
+                  <c:v>Potash</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Potash</c:v>
+                  <c:v>Saltpeter</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>Saltpeter</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>Posphorite</c:v>
                 </c:pt>
               </c:strCache>
@@ -2096,10 +2084,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$I$3:$I$42</c:f>
+              <c:f>Data!$I$3:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2122,102 +2110,99 @@
                   <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>242</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>246</c:v>
+                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>241</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>249</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>230</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>249</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>252</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>249</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>75</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>70</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>81</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>56</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>146</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>83</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>254</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>255</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>79</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>38</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>21</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>250</c:v>
-                </c:pt>
                 <c:pt idx="37">
-                  <c:v>150</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
@@ -2247,8 +2232,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="362214184"/>
-        <c:axId val="362213008"/>
+        <c:axId val="308114168"/>
+        <c:axId val="308119656"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2331,7 +2316,6 @@
                   <c:showLeaderLines val="0"/>
                   <c:extLst>
                     <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:layout/>
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
                         <c:spPr>
@@ -2354,12 +2338,12 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Data!$G$3:$G$42</c15:sqref>
+                          <c15:sqref>Data!$G$3:$G$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="40"/>
+                      <c:ptCount val="39"/>
                       <c:pt idx="0">
                         <c:v>Copper</c:v>
                       </c:pt>
@@ -2382,102 +2366,99 @@
                         <c:v>Fe-Cu-Sn Mix</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>Mana Infused</c:v>
+                        <c:v>Prometheum</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>Prometheum</c:v>
+                        <c:v>Deep Iron</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>Deep Iron</c:v>
+                        <c:v>Infuscolium</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>Infuscolium</c:v>
+                        <c:v>Oureclase</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>Oureclase</c:v>
+                        <c:v>Astral Silver</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>Astral Silver</c:v>
+                        <c:v>Carmot</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>Carmot</c:v>
+                        <c:v>Mithril</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>Mithril</c:v>
+                        <c:v>Rubracium</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>Rubracium</c:v>
+                        <c:v>Orichalcum</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>Orichalcum</c:v>
+                        <c:v>Adamantine</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>Adamantine</c:v>
+                        <c:v>Atlarus</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>Atlarus</c:v>
+                        <c:v>Platinum</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>Platinum</c:v>
+                        <c:v>Zinc</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>Zinc</c:v>
+                        <c:v>Certus Quartz</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>Certus Quartz</c:v>
+                        <c:v>Aluminum</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>Aluminum</c:v>
+                        <c:v>Manganese</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>Manganese</c:v>
+                        <c:v>Sulfur - Veins</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>Sulfur - Veins</c:v>
+                        <c:v>Sulfur - Deposits</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>Sulfur - Deposits</c:v>
+                        <c:v>Apatite</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>Apatite</c:v>
+                        <c:v>Salt</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>Salt</c:v>
+                        <c:v>Coal</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>Coal</c:v>
+                        <c:v>Iron</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>Iron</c:v>
+                        <c:v>Gold</c:v>
                       </c:pt>
                       <c:pt idx="30">
-                        <c:v>Gold</c:v>
+                        <c:v>Redstone</c:v>
                       </c:pt>
                       <c:pt idx="31">
-                        <c:v>Redstone</c:v>
+                        <c:v>Diamond</c:v>
                       </c:pt>
                       <c:pt idx="32">
-                        <c:v>Diamond</c:v>
+                        <c:v>Lapis</c:v>
                       </c:pt>
                       <c:pt idx="33">
-                        <c:v>Lapis</c:v>
+                        <c:v>Emerald</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>Emerald</c:v>
+                        <c:v>Magnesium</c:v>
                       </c:pt>
                       <c:pt idx="35">
-                        <c:v>Magnesium</c:v>
+                        <c:v>Bitumen</c:v>
                       </c:pt>
                       <c:pt idx="36">
-                        <c:v>Bitumen</c:v>
+                        <c:v>Potash</c:v>
                       </c:pt>
                       <c:pt idx="37">
-                        <c:v>Potash</c:v>
+                        <c:v>Saltpeter</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>Saltpeter</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
                         <c:v>Posphorite</c:v>
                       </c:pt>
                     </c:strCache>
@@ -2488,13 +2469,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Data!$J$3:$J$42</c15:sqref>
+                          <c15:sqref>Data!$J$3:$J$41</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="40"/>
+                      <c:ptCount val="39"/>
                       <c:pt idx="0">
                         <c:v>75</c:v>
                       </c:pt>
@@ -2517,102 +2498,99 @@
                         <c:v>169</c:v>
                       </c:pt>
                       <c:pt idx="7">
+                        <c:v>228.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>234.5</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>224.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>228.5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>242</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>243</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>235.5</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>219</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>239.5</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>247</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>241.5</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>62.5</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>141</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>157</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>139.5</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
                         <c:v>20</c:v>
                       </c:pt>
-                      <c:pt idx="8">
-                        <c:v>228.5</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>234.5</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>224.5</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>228.5</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>242</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>243</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>233</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>219</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>239.5</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>247</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>241.5</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>65</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>53</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>62.5</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>40</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>141</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>64</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>157</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>139.5</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>62</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>11</c:v>
-                      </c:pt>
                       <c:pt idx="33">
-                        <c:v>20</c:v>
+                        <c:v>11.5</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>11.5</c:v>
+                        <c:v>127.5</c:v>
                       </c:pt>
                       <c:pt idx="35">
+                        <c:v>177.5</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
                         <c:v>127.5</c:v>
                       </c:pt>
-                      <c:pt idx="36">
-                        <c:v>177.5</c:v>
-                      </c:pt>
                       <c:pt idx="37">
-                        <c:v>127.5</c:v>
+                        <c:v>69</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>69</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
                         <c:v>110</c:v>
                       </c:pt>
                     </c:numCache>
@@ -2625,7 +2603,7 @@
         </c:extLst>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="362214184"/>
+        <c:axId val="308114168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,7 +2660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362213008"/>
+        <c:crossAx val="308119656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2690,7 +2668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362213008"/>
+        <c:axId val="308119656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -2757,7 +2735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362214184"/>
+        <c:crossAx val="308114168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="32"/>
@@ -4324,7 +4302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -4335,10 +4313,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4435,7 +4413,7 @@
         <v>66</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J42" si="0">AVERAGE(H4:I4)</f>
+        <f t="shared" ref="J4:J9" si="0">AVERAGE(H4:I4)</f>
         <v>48</v>
       </c>
     </row>
@@ -4597,14 +4575,14 @@
         <v>39</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="I10">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>AVERAGE(H10:I10)</f>
+        <v>228.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4625,14 +4603,14 @@
         <v>40</v>
       </c>
       <c r="H11">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="I11">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>228.5</v>
+        <f>AVERAGE(H11:I11)</f>
+        <v>234.5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4653,14 +4631,14 @@
         <v>41</v>
       </c>
       <c r="H12">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I12">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
-        <v>234.5</v>
+        <f>AVERAGE(H12:I12)</f>
+        <v>224.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -4684,11 +4662,11 @@
         <v>208</v>
       </c>
       <c r="I13">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
-        <v>224.5</v>
+        <f>AVERAGE(H13:I13)</f>
+        <v>228.5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4709,14 +4687,14 @@
         <v>43</v>
       </c>
       <c r="H14">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="I14">
         <v>249</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
-        <v>228.5</v>
+        <f>AVERAGE(H14:I14)</f>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -4740,11 +4718,11 @@
         <v>235</v>
       </c>
       <c r="I15">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
-        <v>242</v>
+        <f>AVERAGE(H15:I15)</f>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -4765,14 +4743,14 @@
         <v>45</v>
       </c>
       <c r="H16">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="I16">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
-        <v>243</v>
+        <f>AVERAGE(H16:I16)</f>
+        <v>235.5</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4793,14 +4771,14 @@
         <v>46</v>
       </c>
       <c r="H17">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="I17">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
-        <v>233</v>
+        <f>AVERAGE(H17:I17)</f>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -4821,14 +4799,14 @@
         <v>47</v>
       </c>
       <c r="H18">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="I18">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
-        <v>219</v>
+        <f>AVERAGE(H18:I18)</f>
+        <v>239.5</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -4849,14 +4827,14 @@
         <v>48</v>
       </c>
       <c r="H19">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="I19">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
-        <v>239.5</v>
+        <f>AVERAGE(H19:I19)</f>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -4877,14 +4855,14 @@
         <v>49</v>
       </c>
       <c r="H20">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="I20">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
-        <v>247</v>
+        <f>AVERAGE(H20:I20)</f>
+        <v>241.5</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -4902,17 +4880,17 @@
         <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H21">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <v>249</v>
+        <v>10</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
-        <v>241.5</v>
+        <f>AVERAGE(H21:I21)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -4930,17 +4908,17 @@
         <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="I22">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>AVERAGE(H22:I22)</f>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -4961,14 +4939,14 @@
         <v>51</v>
       </c>
       <c r="H23">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="I23">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f>AVERAGE(H23:I23)</f>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4989,14 +4967,14 @@
         <v>52</v>
       </c>
       <c r="H24">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I24">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>AVERAGE(H24:I24)</f>
+        <v>62.5</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -5017,14 +4995,14 @@
         <v>53</v>
       </c>
       <c r="H25">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="I25">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
-        <v>62.5</v>
+        <f>AVERAGE(H25:I25)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -5045,14 +5023,14 @@
         <v>54</v>
       </c>
       <c r="H26">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="I26">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>AVERAGE(H26:I26)</f>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -5073,14 +5051,14 @@
         <v>55</v>
       </c>
       <c r="H27">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="I27">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
-        <v>141</v>
+        <f>AVERAGE(H27:I27)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -5101,14 +5079,14 @@
         <v>56</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="I28">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>AVERAGE(H28:I28)</f>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -5129,14 +5107,14 @@
         <v>57</v>
       </c>
       <c r="H29">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="I29">
-        <v>83</v>
+        <v>254</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <f>AVERAGE(H29:I29)</f>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -5157,14 +5135,14 @@
         <v>58</v>
       </c>
       <c r="H30">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="I30">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
-        <v>157</v>
+        <f>AVERAGE(H30:I30)</f>
+        <v>139.5</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -5172,14 +5150,14 @@
         <v>59</v>
       </c>
       <c r="H31">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="I31">
-        <v>255</v>
+        <v>79</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
-        <v>139.5</v>
+        <f>AVERAGE(H31:I31)</f>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -5187,14 +5165,14 @@
         <v>60</v>
       </c>
       <c r="H32">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I32">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <f>AVERAGE(H32:I32)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
@@ -5202,14 +5180,14 @@
         <v>61</v>
       </c>
       <c r="H33">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I33">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>AVERAGE(H33:I33)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
@@ -5217,14 +5195,14 @@
         <v>62</v>
       </c>
       <c r="H34">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I34">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>AVERAGE(H34:I34)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
@@ -5235,11 +5213,11 @@
         <v>2</v>
       </c>
       <c r="I35">
+        <v>38</v>
+      </c>
+      <c r="J35">
+        <f>AVERAGE(H35:I35)</f>
         <v>20</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>11</v>
       </c>
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
@@ -5250,41 +5228,41 @@
         <v>2</v>
       </c>
       <c r="I36">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="J36">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>AVERAGE(H36:I36)</f>
+        <v>11.5</v>
       </c>
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="I37">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="J37">
-        <f t="shared" si="0"/>
-        <v>11.5</v>
+        <f>AVERAGE(H37:I37)</f>
+        <v>127.5</v>
       </c>
     </row>
     <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="H38">
         <v>105</v>
       </c>
       <c r="I38">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="J38">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
+        <f>AVERAGE(H38:I38)</f>
+        <v>177.5</v>
       </c>
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
@@ -5295,11 +5273,11 @@
         <v>105</v>
       </c>
       <c r="I39">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="J39">
-        <f t="shared" si="0"/>
-        <v>177.5</v>
+        <f>AVERAGE(H39:I39)</f>
+        <v>127.5</v>
       </c>
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
@@ -5307,14 +5285,14 @@
         <v>67</v>
       </c>
       <c r="H40">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="I40">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
+        <f>AVERAGE(H40:I40)</f>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
@@ -5322,28 +5300,13 @@
         <v>68</v>
       </c>
       <c r="H41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="I41">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J41">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G42" t="s">
-        <v>69</v>
-      </c>
-      <c r="H42">
-        <v>85</v>
-      </c>
-      <c r="I42">
-        <v>135</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H41:I41)</f>
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Overworld ore distribution to document
</commit_message>
<xml_diff>
--- a/Documents/OreDistribution.xlsx
+++ b/Documents/OreDistribution.xlsx
@@ -14,7 +14,9 @@
   <sheets>
     <sheet name="Nether" sheetId="2" r:id="rId1"/>
     <sheet name="Deep Dark" sheetId="3" r:id="rId2"/>
-    <sheet name="Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Overworld" sheetId="4" r:id="rId3"/>
+    <sheet name="Overworld - Magical" sheetId="5" r:id="rId4"/>
+    <sheet name="Data" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -234,6 +236,12 @@
   <si>
     <t>Posphorite</t>
   </si>
+  <si>
+    <t>Overworld</t>
+  </si>
+  <si>
+    <t>Overworld - Magical</t>
+  </si>
 </sst>
 </file>
 
@@ -959,8 +967,8 @@
             </c:spPr>
           </c:downBars>
         </c:upDownBars>
-        <c:axId val="308118872"/>
-        <c:axId val="308116912"/>
+        <c:axId val="263420840"/>
+        <c:axId val="263425936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1264,7 +1272,7 @@
         </c:extLst>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="308118872"/>
+        <c:axId val="263420840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308116912"/>
+        <c:crossAx val="263425936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1329,7 +1337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308116912"/>
+        <c:axId val="263425936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="128"/>
@@ -1393,7 +1401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308118872"/>
+        <c:crossAx val="263420840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="32"/>
@@ -2232,8 +2240,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="308114168"/>
-        <c:axId val="308119656"/>
+        <c:axId val="263426328"/>
+        <c:axId val="263424368"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2603,7 +2611,7 @@
         </c:extLst>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="308114168"/>
+        <c:axId val="263426328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,7 +2668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308119656"/>
+        <c:crossAx val="263424368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2668,7 +2676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308119656"/>
+        <c:axId val="263424368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -2735,7 +2743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308114168"/>
+        <c:crossAx val="263426328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="32"/>
@@ -2765,6 +2773,1944 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
         </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Overworld</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$L$3:$L$30</c:f>
+              <c:strCache>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>Copper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Silver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lead</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Nickel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Osmium</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fe-Cu-Sn Mix</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Platinum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Zinc</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Certus Quartz</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Aluminum</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Manganese</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sulfur - Veins</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sulfur - Deposits</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Apatite</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Salt</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Coal</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Iron</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Gold</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Redstone</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Diamond</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Lapis</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Emerald</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Magnesium</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Bitumen</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Potash</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Saltpeter</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Posphorite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$M$3:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$L$3:$L$30</c:f>
+              <c:strCache>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>Copper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Silver</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lead</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Nickel</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Osmium</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fe-Cu-Sn Mix</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Platinum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Zinc</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Certus Quartz</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Aluminum</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Manganese</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sulfur - Veins</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sulfur - Deposits</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Apatite</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Salt</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Coal</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Iron</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Gold</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Redstone</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Diamond</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Lapis</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Emerald</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Magnesium</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Bitumen</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Potash</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Saltpeter</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Posphorite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$3:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="261311256"/>
+        <c:axId val="263422016"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$O$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Mean</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$L$3:$L$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="28"/>
+                      <c:pt idx="0">
+                        <c:v>Copper</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Tin</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Silver</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lead</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Nickel</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Osmium</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Fe-Cu-Sn Mix</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Platinum</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Zinc</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Certus Quartz</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>Aluminum</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Manganese</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>Sulfur - Veins</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>Sulfur - Deposits</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>Apatite</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>Salt</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>Coal</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>Iron</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>Gold</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>Redstone</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>Diamond</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>Lapis</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>Emerald</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>Magnesium</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>Bitumen</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>Potash</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>Saltpeter</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>Posphorite</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$O$3:$O$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="28"/>
+                      <c:pt idx="0">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17.5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>54.5</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>108</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>127.5</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>177.5</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>127.5</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>110</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="261311256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="35000"/>
+                <a:lumOff val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="263422016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="263422016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="260"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261311256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="32"/>
+        <c:minorUnit val="16"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="83000"/>
+                <a:lumOff val="17000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="75000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Overworld - Magical</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$Q$3:$Q$13</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Prometheum</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deep Iron</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Infuscolium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oureclase</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Astral Silver</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Carmot</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mithril</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rubracium</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Orichalcum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adamantine</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Atlarus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$R$3:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$Q$3:$Q$13</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Prometheum</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deep Iron</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Infuscolium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Oureclase</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Astral Silver</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Carmot</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mithril</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rubracium</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Orichalcum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adamantine</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Atlarus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$S$3:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="438744952"/>
+        <c:axId val="438750440"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$T$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Mean</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$Q$3:$Q$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>Prometheum</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Deep Iron</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Infuscolium</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Oureclase</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Astral Silver</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Carmot</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Mithril</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rubracium</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Orichalcum</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Adamantine</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>Atlarus</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$T$3:$T$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>14.5</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="438744952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="35000"/>
+                <a:lumOff val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438750440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="438750440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="64"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438744952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="32"/>
+        <c:minorUnit val="8"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -2888,6 +4834,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
   <cs:axisTitle>
@@ -3420,6 +5446,1068 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="10000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="331">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3988,6 +7076,80 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4313,10 +7475,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T41"/>
+  <sheetViews>
+    <sheetView topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4325,17 +7515,25 @@
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4360,8 +7558,32 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4388,8 +7610,34 @@
         <f>AVERAGE(H3:I3)</f>
         <v>75</v>
       </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3">
+        <v>51</v>
+      </c>
+      <c r="N3">
+        <v>65</v>
+      </c>
+      <c r="O3">
+        <f>AVERAGE(M3:N3)</f>
+        <v>58</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>30</v>
+      </c>
+      <c r="T3">
+        <f>AVERAGE(R3:S3)</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4416,8 +7664,34 @@
         <f t="shared" ref="J4:J9" si="0">AVERAGE(H4:I4)</f>
         <v>48</v>
       </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4">
+        <v>23</v>
+      </c>
+      <c r="N4">
+        <v>51</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O41" si="1">AVERAGE(M4:N4)</f>
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4">
+        <v>12</v>
+      </c>
+      <c r="S4">
+        <v>24</v>
+      </c>
+      <c r="T4">
+        <f>AVERAGE(R4:S4)</f>
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4444,8 +7718,34 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5">
+        <v>18</v>
+      </c>
+      <c r="N5">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5">
+        <v>20</v>
+      </c>
+      <c r="S5">
+        <v>32</v>
+      </c>
+      <c r="T5">
+        <f>AVERAGE(R5:S5)</f>
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4472,8 +7772,34 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>34</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6">
+        <v>10</v>
+      </c>
+      <c r="S6">
+        <v>36</v>
+      </c>
+      <c r="T6">
+        <f>AVERAGE(R6:S6)</f>
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4484,7 +7810,7 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D30" si="1">AVERAGE(B7:C7)</f>
+        <f t="shared" ref="D7:D30" si="2">AVERAGE(B7:C7)</f>
         <v>32</v>
       </c>
       <c r="G7" t="s">
@@ -4500,8 +7826,34 @@
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>27</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7">
+        <v>10</v>
+      </c>
+      <c r="S7">
+        <v>16</v>
+      </c>
+      <c r="T7">
+        <f>AVERAGE(R7:S7)</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4512,7 +7864,7 @@
         <v>54</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="G8" t="s">
@@ -4528,8 +7880,34 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>30</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+      <c r="T8">
+        <f>AVERAGE(R8:S8)</f>
+        <v>7.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4540,7 +7918,7 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G9" t="s">
@@ -4556,8 +7934,34 @@
         <f t="shared" si="0"/>
         <v>169</v>
       </c>
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9">
+        <v>64</v>
+      </c>
+      <c r="N9">
+        <v>192</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>45</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>23</v>
+      </c>
+      <c r="T9">
+        <f>AVERAGE(R9:S9)</f>
+        <v>14</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4568,7 +7972,7 @@
         <v>68</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="G10" t="s">
@@ -4581,11 +7985,37 @@
         <v>242</v>
       </c>
       <c r="J10">
-        <f>AVERAGE(H10:I10)</f>
+        <f t="shared" ref="J10:J41" si="3">AVERAGE(H10:I10)</f>
         <v>228.5</v>
       </c>
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <f>AVERAGE(M10:N10)</f>
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10">
+        <v>28</v>
+      </c>
+      <c r="S10">
+        <v>36</v>
+      </c>
+      <c r="T10">
+        <f>AVERAGE(R10:S10)</f>
+        <v>32</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4596,7 +8026,7 @@
         <v>60</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="G11" t="s">
@@ -4609,11 +8039,37 @@
         <v>246</v>
       </c>
       <c r="J11">
-        <f>AVERAGE(H11:I11)</f>
+        <f t="shared" si="3"/>
         <v>234.5</v>
       </c>
+      <c r="L11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>42</v>
+      </c>
+      <c r="N11">
+        <v>58</v>
+      </c>
+      <c r="O11">
+        <f>AVERAGE(M11:N11)</f>
+        <v>50</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <v>19</v>
+      </c>
+      <c r="T11">
+        <f>AVERAGE(R11:S11)</f>
+        <v>14.5</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -4624,7 +8080,7 @@
         <v>32</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G12" t="s">
@@ -4637,11 +8093,37 @@
         <v>241</v>
       </c>
       <c r="J12">
-        <f>AVERAGE(H12:I12)</f>
+        <f t="shared" si="3"/>
         <v>224.5</v>
       </c>
+      <c r="L12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12">
+        <v>36</v>
+      </c>
+      <c r="N12">
+        <v>54</v>
+      </c>
+      <c r="O12">
+        <f>AVERAGE(M12:N12)</f>
+        <v>45</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <f>AVERAGE(R12:S12)</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4652,7 +8134,7 @@
         <v>102</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
       <c r="G13" t="s">
@@ -4665,11 +8147,37 @@
         <v>249</v>
       </c>
       <c r="J13">
-        <f>AVERAGE(H13:I13)</f>
+        <f t="shared" si="3"/>
         <v>228.5</v>
       </c>
+      <c r="L13" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13">
+        <v>44</v>
+      </c>
+      <c r="N13">
+        <v>62</v>
+      </c>
+      <c r="O13">
+        <f>AVERAGE(M13:N13)</f>
+        <v>53</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>16</v>
+      </c>
+      <c r="T13">
+        <f>AVERAGE(R13:S13)</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4680,7 +8188,7 @@
         <v>126</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="G14" t="s">
@@ -4693,11 +8201,24 @@
         <v>249</v>
       </c>
       <c r="J14">
-        <f>AVERAGE(H14:I14)</f>
+        <f t="shared" si="3"/>
         <v>242</v>
       </c>
+      <c r="L14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14">
+        <v>18</v>
+      </c>
+      <c r="N14">
+        <v>42</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(M14:N14)</f>
+        <v>30</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -4708,7 +8229,7 @@
         <v>56</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="G15" t="s">
@@ -4721,11 +8242,24 @@
         <v>251</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(H15:I15)</f>
+        <f t="shared" si="3"/>
         <v>243</v>
       </c>
+      <c r="L15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15">
+        <v>80</v>
+      </c>
+      <c r="N15">
+        <v>88</v>
+      </c>
+      <c r="O15">
+        <f>AVERAGE(M15:N15)</f>
+        <v>84</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4736,7 +8270,7 @@
         <v>58</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G16" t="s">
@@ -4749,11 +8283,24 @@
         <v>250</v>
       </c>
       <c r="J16">
-        <f>AVERAGE(H16:I16)</f>
+        <f t="shared" si="3"/>
         <v>235.5</v>
       </c>
+      <c r="L16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <f>AVERAGE(M16:N16)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -4764,7 +8311,7 @@
         <v>122</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="G17" t="s">
@@ -4777,11 +8324,24 @@
         <v>230</v>
       </c>
       <c r="J17">
-        <f>AVERAGE(H17:I17)</f>
+        <f t="shared" si="3"/>
         <v>219</v>
       </c>
+      <c r="L17" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17">
+        <v>45</v>
+      </c>
+      <c r="N17">
+        <v>64</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(M17:N17)</f>
+        <v>54.5</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -4792,7 +8352,7 @@
         <v>48</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="G18" t="s">
@@ -4805,11 +8365,24 @@
         <v>249</v>
       </c>
       <c r="J18">
-        <f>AVERAGE(H18:I18)</f>
+        <f t="shared" si="3"/>
         <v>239.5</v>
       </c>
+      <c r="L18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18">
+        <v>60</v>
+      </c>
+      <c r="N18">
+        <v>120</v>
+      </c>
+      <c r="O18">
+        <f>AVERAGE(M18:N18)</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -4820,7 +8393,7 @@
         <v>32</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G19" t="s">
@@ -4833,11 +8406,24 @@
         <v>252</v>
       </c>
       <c r="J19">
-        <f>AVERAGE(H19:I19)</f>
+        <f t="shared" si="3"/>
         <v>247</v>
       </c>
+      <c r="L19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19">
+        <v>24</v>
+      </c>
+      <c r="N19">
+        <v>192</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(M19:N19)</f>
+        <v>108</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -4848,7 +8434,7 @@
         <v>126</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="G20" t="s">
@@ -4861,11 +8447,24 @@
         <v>249</v>
       </c>
       <c r="J20">
-        <f>AVERAGE(H20:I20)</f>
+        <f t="shared" si="3"/>
         <v>241.5</v>
       </c>
+      <c r="L20" t="s">
+        <v>59</v>
+      </c>
+      <c r="M20">
+        <v>35</v>
+      </c>
+      <c r="N20">
+        <v>61</v>
+      </c>
+      <c r="O20">
+        <f>AVERAGE(M20:N20)</f>
+        <v>48</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -4876,7 +8475,7 @@
         <v>66</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="G21" t="s">
@@ -4889,11 +8488,24 @@
         <v>10</v>
       </c>
       <c r="J21">
-        <f>AVERAGE(H21:I21)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21">
+        <v>12</v>
+      </c>
+      <c r="N21">
+        <v>24</v>
+      </c>
+      <c r="O21">
+        <f>AVERAGE(M21:N21)</f>
+        <v>18</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -4904,7 +8516,7 @@
         <v>52</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="G22" t="s">
@@ -4917,11 +8529,24 @@
         <v>75</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(H22:I22)</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
+      <c r="L22" t="s">
+        <v>61</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>18</v>
+      </c>
+      <c r="O22">
+        <f>AVERAGE(M22:N22)</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4932,7 +8557,7 @@
         <v>66</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="G23" t="s">
@@ -4945,11 +8570,24 @@
         <v>70</v>
       </c>
       <c r="J23">
-        <f>AVERAGE(H23:I23)</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
+      <c r="L23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>16</v>
+      </c>
+      <c r="O23">
+        <f>AVERAGE(M23:N23)</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -4960,7 +8598,7 @@
         <v>76</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="G24" t="s">
@@ -4973,11 +8611,24 @@
         <v>81</v>
       </c>
       <c r="J24">
-        <f>AVERAGE(H24:I24)</f>
+        <f t="shared" si="3"/>
         <v>62.5</v>
       </c>
+      <c r="L24" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>29</v>
+      </c>
+      <c r="O24">
+        <f>AVERAGE(M24:N24)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -4988,7 +8639,7 @@
         <v>122</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63.5</v>
       </c>
       <c r="G25" t="s">
@@ -5001,11 +8652,24 @@
         <v>56</v>
       </c>
       <c r="J25">
-        <f>AVERAGE(H25:I25)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
+      <c r="L25" t="s">
+        <v>64</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>16</v>
+      </c>
+      <c r="O25">
+        <f>AVERAGE(M25:N25)</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -5016,7 +8680,7 @@
         <v>66</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="G26" t="s">
@@ -5029,11 +8693,24 @@
         <v>146</v>
       </c>
       <c r="J26">
-        <f>AVERAGE(H26:I26)</f>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
+      <c r="L26" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>105</v>
+      </c>
+      <c r="N26">
+        <v>150</v>
+      </c>
+      <c r="O26">
+        <f>AVERAGE(M26:N26)</f>
+        <v>127.5</v>
+      </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -5044,7 +8721,7 @@
         <v>52</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="G27" t="s">
@@ -5057,11 +8734,24 @@
         <v>13</v>
       </c>
       <c r="J27">
-        <f>AVERAGE(H27:I27)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
+      <c r="L27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27">
+        <v>105</v>
+      </c>
+      <c r="N27">
+        <v>250</v>
+      </c>
+      <c r="O27">
+        <f>AVERAGE(M27:N27)</f>
+        <v>177.5</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5072,7 +8762,7 @@
         <v>66</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="G28" t="s">
@@ -5085,11 +8775,24 @@
         <v>83</v>
       </c>
       <c r="J28">
-        <f>AVERAGE(H28:I28)</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
+      <c r="L28" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28">
+        <v>105</v>
+      </c>
+      <c r="N28">
+        <v>150</v>
+      </c>
+      <c r="O28">
+        <f>AVERAGE(M28:N28)</f>
+        <v>127.5</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -5100,7 +8803,7 @@
         <v>38</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.5</v>
       </c>
       <c r="G29" t="s">
@@ -5113,11 +8816,24 @@
         <v>254</v>
       </c>
       <c r="J29">
-        <f>AVERAGE(H29:I29)</f>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
+      <c r="L29" t="s">
+        <v>67</v>
+      </c>
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="N29">
+        <v>128</v>
+      </c>
+      <c r="O29">
+        <f>AVERAGE(M29:N29)</f>
+        <v>69</v>
+      </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -5128,7 +8844,7 @@
         <v>24</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G30" t="s">
@@ -5141,11 +8857,24 @@
         <v>255</v>
       </c>
       <c r="J30">
-        <f>AVERAGE(H30:I30)</f>
+        <f t="shared" si="3"/>
         <v>139.5</v>
       </c>
+      <c r="L30" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30">
+        <v>85</v>
+      </c>
+      <c r="N30">
+        <v>135</v>
+      </c>
+      <c r="O30">
+        <f>AVERAGE(M30:N30)</f>
+        <v>110</v>
+      </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>59</v>
       </c>
@@ -5156,11 +8885,11 @@
         <v>79</v>
       </c>
       <c r="J31">
-        <f>AVERAGE(H31:I31)</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>60</v>
       </c>
@@ -5171,7 +8900,7 @@
         <v>31</v>
       </c>
       <c r="J32">
-        <f>AVERAGE(H32:I32)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
@@ -5186,7 +8915,7 @@
         <v>23</v>
       </c>
       <c r="J33">
-        <f>AVERAGE(H33:I33)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
@@ -5201,7 +8930,7 @@
         <v>20</v>
       </c>
       <c r="J34">
-        <f>AVERAGE(H34:I34)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
@@ -5216,7 +8945,7 @@
         <v>38</v>
       </c>
       <c r="J35">
-        <f>AVERAGE(H35:I35)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -5231,7 +8960,7 @@
         <v>21</v>
       </c>
       <c r="J36">
-        <f>AVERAGE(H36:I36)</f>
+        <f t="shared" si="3"/>
         <v>11.5</v>
       </c>
     </row>
@@ -5246,7 +8975,7 @@
         <v>150</v>
       </c>
       <c r="J37">
-        <f>AVERAGE(H37:I37)</f>
+        <f t="shared" si="3"/>
         <v>127.5</v>
       </c>
     </row>
@@ -5261,7 +8990,7 @@
         <v>250</v>
       </c>
       <c r="J38">
-        <f>AVERAGE(H38:I38)</f>
+        <f t="shared" si="3"/>
         <v>177.5</v>
       </c>
     </row>
@@ -5276,7 +9005,7 @@
         <v>150</v>
       </c>
       <c r="J39">
-        <f>AVERAGE(H39:I39)</f>
+        <f t="shared" si="3"/>
         <v>127.5</v>
       </c>
     </row>
@@ -5291,7 +9020,7 @@
         <v>128</v>
       </c>
       <c r="J40">
-        <f>AVERAGE(H40:I40)</f>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
     </row>
@@ -5306,7 +9035,7 @@
         <v>135</v>
       </c>
       <c r="J41">
-        <f>AVERAGE(H41:I41)</f>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
     </row>

</xml_diff>